<commit_message>
add integration test for room controller
</commit_message>
<xml_diff>
--- a/docs/SSNoC REST API.xlsx
+++ b/docs/SSNoC REST API.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24760" windowHeight="15600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Guidelines and Notes" sheetId="1" r:id="rId1"/>
@@ -887,30 +887,30 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1263,12 +1263,12 @@
       <c r="D11" s="5"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1">
       <c r="A15" s="43" t="s">
@@ -1295,9 +1295,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y951"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1361,48 +1361,48 @@
       <c r="Y1" s="35"/>
     </row>
     <row r="2" spans="1:25" ht="12">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="49"/>
+      <c r="E2" s="51"/>
       <c r="F2" s="10" t="s">
         <v>28</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49" t="s">
+      <c r="H2" s="51"/>
+      <c r="I2" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="47" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="24" customHeight="1">
-      <c r="A3" s="47"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
       <c r="F3" s="12" t="s">
         <v>32</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
     </row>
     <row r="4" spans="1:25" ht="12">
       <c r="A4" s="14" t="s">
@@ -1553,7 +1553,7 @@
       <c r="I8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="49"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -1592,7 +1592,7 @@
       <c r="I9" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="J9" s="47"/>
+      <c r="J9" s="50"/>
       <c r="K9" s="37"/>
       <c r="L9" s="37"/>
       <c r="M9" s="37"/>
@@ -1934,29 +1934,29 @@
       <c r="Y17" s="3"/>
     </row>
     <row r="18" spans="1:25" ht="12">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="48" t="s">
+      <c r="D18" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="E18" s="51"/>
+      <c r="E18" s="54"/>
       <c r="F18" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="G18" s="49" t="s">
+      <c r="G18" s="51" t="s">
         <v>29</v>
       </c>
       <c r="H18" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="I18" s="48" t="s">
+      <c r="I18" s="53" t="s">
         <v>79</v>
       </c>
       <c r="J18" s="36"/>
@@ -1977,15 +1977,15 @@
       <c r="Y18" s="37"/>
     </row>
     <row r="19" spans="1:25" ht="12">
-      <c r="A19" s="47"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50"/>
       <c r="J19" s="36"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -2159,10 +2159,10 @@
       <c r="A24" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="55" t="s">
+      <c r="C24" s="44" t="s">
         <v>151</v>
       </c>
       <c r="D24" s="5"/>
@@ -2185,10 +2185,10 @@
       <c r="A25" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B25" s="55" t="s">
+      <c r="B25" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="55" t="s">
+      <c r="C25" s="44" t="s">
         <v>155</v>
       </c>
       <c r="D25" s="5"/>
@@ -2211,10 +2211,10 @@
       <c r="A26" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B26" s="55" t="s">
+      <c r="B26" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="55" t="s">
+      <c r="C26" s="44" t="s">
         <v>158</v>
       </c>
       <c r="D26" s="5" t="s">
@@ -2241,10 +2241,10 @@
       <c r="A27" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B27" s="55" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="55" t="s">
+      <c r="B27" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="44" t="s">
         <v>158</v>
       </c>
       <c r="D27" s="5" t="s">
@@ -2279,10 +2279,10 @@
       <c r="A29" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B29" s="55" t="s">
+      <c r="B29" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="55" t="s">
+      <c r="C29" s="44" t="s">
         <v>165</v>
       </c>
       <c r="D29" s="5"/>
@@ -2305,10 +2305,10 @@
       <c r="A30" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B30" s="55" t="s">
+      <c r="B30" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="55" t="s">
+      <c r="C30" s="44" t="s">
         <v>165</v>
       </c>
       <c r="D30" s="5" t="s">
@@ -2335,10 +2335,10 @@
       <c r="A31" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B31" s="55" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="55" t="s">
+      <c r="B31" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="44" t="s">
         <v>165</v>
       </c>
       <c r="D31" s="5" t="s">
@@ -2377,10 +2377,10 @@
       <c r="A33" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B33" s="55" t="s">
+      <c r="B33" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="55" t="s">
+      <c r="C33" s="44" t="s">
         <v>175</v>
       </c>
       <c r="D33" s="5"/>
@@ -2403,10 +2403,10 @@
       <c r="A34" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B34" s="55" t="s">
+      <c r="B34" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="55" t="s">
+      <c r="C34" s="44" t="s">
         <v>178</v>
       </c>
       <c r="D34" s="5"/>
@@ -11570,6 +11570,17 @@
     <row r="951" spans="1:10" ht="12"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="J8:J9"/>
     <mergeCell ref="G18:G19"/>
@@ -11577,17 +11588,6 @@
     <mergeCell ref="H18:H19"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="I18:I19"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C18:C19"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -11937,10 +11937,10 @@
       <c r="D5" s="3"/>
     </row>
     <row r="7" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="45"/>
+      <c r="B7" s="46"/>
     </row>
     <row r="11" spans="1:24" ht="15.75" customHeight="1">
       <c r="C11" s="5"/>

</xml_diff>

<commit_message>
add new features and test cases
</commit_message>
<xml_diff>
--- a/docs/SSNoC REST API.xlsx
+++ b/docs/SSNoC REST API.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26101"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kid7st/Dropbox/myCoding/ECE2016Spring/18652/S16-A2-SSNoC/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengyu/Documents/S16-A2-SSNoC/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15520" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="660" yWindow="460" windowWidth="24940" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Guidelines and Notes" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,6 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -33,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="238">
   <si>
     <t>Rules</t>
   </si>
@@ -258,7 +255,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
       </rPr>
       <t xml:space="preserve">author, </t>
     </r>
@@ -266,7 +262,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <charset val="134"/>
       </rPr>
       <t>content, postedAt</t>
     </r>
@@ -687,6 +682,129 @@
   </si>
   <si>
     <t>Dashboard</t>
+  </si>
+  <si>
+    <t>User History</t>
+  </si>
+  <si>
+    <t>/userhistory/:username</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>an array of histories, each is {timestamp: date, username: string, type: int, content: string}. For type: 1 represents log in/out event; 2 represents change status event; 3 represents chat public event; 4 represents post announcement event</t>
+  </si>
+  <si>
+    <t>Not login: 401</t>
+  </si>
+  <si>
+    <t>upload image</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>post</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>/image</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>image file</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Error 404</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>/announcements</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Administrator Profile</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Administrator Profile</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Profile</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>/profile/:username</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Profile Page</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>/profile/</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>username, status, avatar, company, gender, location, email, phone</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Error 401: No user exists</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Profile Page</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>/admin/:userid</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>username, password, account status(active, or inactive), privilege. The password could be empty if you don’t want to modify the password</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>No privilege:  441, Invalid Input: 403</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>An json of users's profile. Including username, status, avatar, company, gender, location, email, phone，</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -705,50 +823,42 @@
       <u/>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
       <i/>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="11"/>
       <name val="Arial"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -915,7 +1025,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1018,6 +1128,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1040,16 +1153,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="已访问的超链接" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1404,12 +1517,12 @@
       <c r="D11" s="5"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="43" t="s">
@@ -1432,9 +1545,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y951"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1498,48 +1611,48 @@
       <c r="Y1" s="35"/>
     </row>
     <row r="2" spans="1:25" ht="13" x14ac:dyDescent="0.15">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="51"/>
+      <c r="E2" s="52"/>
       <c r="F2" s="10" t="s">
         <v>28</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51" t="s">
+      <c r="H2" s="52"/>
+      <c r="I2" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="47" t="s">
+      <c r="J2" s="48" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="50"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
       <c r="F3" s="12" t="s">
         <v>32</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
     </row>
     <row r="4" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
@@ -1690,7 +1803,7 @@
       <c r="I8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="49"/>
+      <c r="J8" s="50"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -1729,7 +1842,7 @@
       <c r="I9" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="J9" s="50"/>
+      <c r="J9" s="51"/>
       <c r="K9" s="37"/>
       <c r="L9" s="37"/>
       <c r="M9" s="37"/>
@@ -1916,7 +2029,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>72</v>
+        <v>217</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>73</v>
@@ -2071,29 +2184,29 @@
       <c r="Y17" s="3"/>
     </row>
     <row r="18" spans="1:25" ht="13" x14ac:dyDescent="0.15">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="53" t="s">
+      <c r="D18" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="E18" s="54"/>
-      <c r="F18" s="52" t="s">
+      <c r="E18" s="55"/>
+      <c r="F18" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="G18" s="51" t="s">
+      <c r="G18" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="52" t="s">
+      <c r="H18" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="I18" s="53" t="s">
+      <c r="I18" s="54" t="s">
         <v>79</v>
       </c>
       <c r="J18" s="36"/>
@@ -2114,15 +2227,15 @@
       <c r="Y18" s="37"/>
     </row>
     <row r="19" spans="1:25" ht="13" x14ac:dyDescent="0.15">
-      <c r="A19" s="50"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
+      <c r="A19" s="51"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
       <c r="J19" s="36"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -2718,54 +2831,146 @@
       <c r="I40" s="5"/>
       <c r="J40" s="40"/>
     </row>
-    <row r="41" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="A41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="5"/>
+    <row r="41" spans="1:10" ht="91" x14ac:dyDescent="0.15">
+      <c r="A41" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B41" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F41" s="33">
+        <v>200</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H41" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>206</v>
+      </c>
       <c r="J41" s="40"/>
     </row>
     <row r="42" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="A42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="A42" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B42" s="44" t="s">
+        <v>212</v>
+      </c>
+      <c r="C42" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="E42" s="5"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="33"/>
-      <c r="I42" s="5"/>
+      <c r="F42" s="33">
+        <v>200</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="H42" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>211</v>
+      </c>
       <c r="J42" s="40"/>
     </row>
-    <row r="43" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="A43" s="5"/>
-      <c r="D43" s="5"/>
+    <row r="43" spans="1:10" ht="52" x14ac:dyDescent="0.15">
+      <c r="A43" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B43" s="44" t="s">
+        <v>221</v>
+      </c>
+      <c r="C43" s="44" t="s">
+        <v>234</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>235</v>
+      </c>
       <c r="E43" s="5"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="5"/>
+      <c r="F43" s="33">
+        <v>200</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="H43" s="33" t="s">
+        <v>236</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>223</v>
+      </c>
       <c r="J43" s="40"/>
     </row>
-    <row r="44" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="A44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="5"/>
+    <row r="44" spans="1:10" ht="39" x14ac:dyDescent="0.15">
+      <c r="A44" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B44" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="C44" s="44" t="s">
+        <v>225</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F44" s="33">
+        <v>200</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>226</v>
+      </c>
       <c r="H44" s="33"/>
-      <c r="I44" s="5"/>
+      <c r="I44" s="5" t="s">
+        <v>227</v>
+      </c>
       <c r="J44" s="40"/>
     </row>
-    <row r="45" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="A45" s="5"/>
-      <c r="D45" s="5"/>
+    <row r="45" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+      <c r="A45" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B45" s="44" t="s">
+        <v>228</v>
+      </c>
+      <c r="C45" s="44" t="s">
+        <v>229</v>
+      </c>
+      <c r="D45" s="45" t="s">
+        <v>230</v>
+      </c>
       <c r="E45" s="5"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="5"/>
+      <c r="F45" s="33">
+        <v>200</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="H45" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>233</v>
+      </c>
       <c r="J45" s="40"/>
     </row>
     <row r="46" spans="1:10" ht="13" x14ac:dyDescent="0.15">
@@ -12155,10 +12360,10 @@
       <c r="D5" s="3"/>
     </row>
     <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="46"/>
+      <c r="B7" s="47"/>
     </row>
     <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C11" s="5"/>

</xml_diff>